<commit_message>
(minor: update xls files to add break trial)
</commit_message>
<xml_diff>
--- a/lists/learn_list_study4_base.xlsx
+++ b/lists/learn_list_study4_base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gelliott/Documents/projects/delaylearn/feedback-delay-four/lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB773C1-53DA-B840-9610-43BB38DFE203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7C335E-8280-8E40-BFDF-19381568A63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2420" yWindow="1240" windowWidth="43380" windowHeight="27560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1108,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E25E4B-9AFA-2443-8C1F-D7B80241CF51}">
-  <dimension ref="A1:AC109"/>
+  <dimension ref="A1:AC115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1:Z115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1300,6 +1300,9 @@
       <c r="Y2">
         <v>1</v>
       </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
       <c r="AA2">
         <v>1</v>
       </c>
@@ -1395,6 +1398,9 @@
       <c r="Y3">
         <v>0</v>
       </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
       <c r="AA3">
         <v>1</v>
       </c>
@@ -1490,6 +1496,9 @@
       <c r="Y4">
         <v>1</v>
       </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
       <c r="AA4">
         <v>2</v>
       </c>
@@ -1586,6 +1595,9 @@
       <c r="Y5">
         <v>0</v>
       </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
       <c r="AA5">
         <v>2</v>
       </c>
@@ -1682,6 +1694,9 @@
       <c r="Y6">
         <v>0</v>
       </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
       <c r="AA6">
         <v>3</v>
       </c>
@@ -1778,6 +1793,9 @@
       <c r="Y7">
         <v>1</v>
       </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
       <c r="AA7">
         <v>3</v>
       </c>
@@ -1874,6 +1892,9 @@
       <c r="Y8">
         <v>1</v>
       </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
       <c r="AA8">
         <v>4</v>
       </c>
@@ -1970,6 +1991,9 @@
       <c r="Y9">
         <v>0</v>
       </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
       <c r="AA9">
         <v>4</v>
       </c>
@@ -2066,6 +2090,9 @@
       <c r="Y10">
         <v>0</v>
       </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
       <c r="AA10">
         <v>5</v>
       </c>
@@ -2162,6 +2189,9 @@
       <c r="Y11">
         <v>1</v>
       </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
       <c r="AA11">
         <v>5</v>
       </c>
@@ -2258,6 +2288,9 @@
       <c r="Y12">
         <v>0</v>
       </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
       <c r="AA12">
         <v>6</v>
       </c>
@@ -2354,6 +2387,9 @@
       <c r="Y13">
         <v>1</v>
       </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
       <c r="AA13">
         <v>6</v>
       </c>
@@ -2450,6 +2486,9 @@
       <c r="Y14">
         <v>0</v>
       </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
       <c r="AA14">
         <v>7</v>
       </c>
@@ -2546,6 +2585,9 @@
       <c r="Y15">
         <v>1</v>
       </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
       <c r="AA15">
         <v>7</v>
       </c>
@@ -2642,6 +2684,9 @@
       <c r="Y16">
         <v>0</v>
       </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
       <c r="AA16">
         <v>8</v>
       </c>
@@ -2738,6 +2783,9 @@
       <c r="Y17">
         <v>1</v>
       </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
       <c r="AA17">
         <v>8</v>
       </c>
@@ -2834,6 +2882,9 @@
       <c r="Y18">
         <v>1</v>
       </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
       <c r="AA18">
         <v>9</v>
       </c>
@@ -2930,6 +2981,9 @@
       <c r="Y19">
         <v>0</v>
       </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
       <c r="AA19">
         <v>9</v>
       </c>
@@ -3026,6 +3080,9 @@
       <c r="Y20">
         <v>0</v>
       </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
       <c r="AA20">
         <v>10</v>
       </c>
@@ -3122,6 +3179,9 @@
       <c r="Y21">
         <v>1</v>
       </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
       <c r="AA21">
         <v>10</v>
       </c>
@@ -3218,6 +3278,9 @@
       <c r="Y22">
         <v>0</v>
       </c>
+      <c r="Z22">
+        <v>0</v>
+      </c>
       <c r="AA22">
         <v>11</v>
       </c>
@@ -3314,6 +3377,9 @@
       <c r="Y23">
         <v>0</v>
       </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
       <c r="AA23">
         <v>12</v>
       </c>
@@ -3410,6 +3476,9 @@
       <c r="Y24">
         <v>1</v>
       </c>
+      <c r="Z24">
+        <v>1</v>
+      </c>
       <c r="AA24">
         <v>11</v>
       </c>
@@ -3506,6 +3575,9 @@
       <c r="Y25">
         <v>1</v>
       </c>
+      <c r="Z25">
+        <v>0</v>
+      </c>
       <c r="AA25">
         <v>12</v>
       </c>
@@ -3602,6 +3674,9 @@
       <c r="Y26">
         <v>1</v>
       </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
       <c r="AA26">
         <v>13</v>
       </c>
@@ -3698,6 +3773,9 @@
       <c r="Y27">
         <v>0</v>
       </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
       <c r="AA27">
         <v>13</v>
       </c>
@@ -3794,6 +3872,9 @@
       <c r="Y28">
         <v>0</v>
       </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
       <c r="AA28">
         <v>14</v>
       </c>
@@ -3890,6 +3971,9 @@
       <c r="Y29">
         <v>1</v>
       </c>
+      <c r="Z29">
+        <v>0</v>
+      </c>
       <c r="AA29">
         <v>14</v>
       </c>
@@ -3986,6 +4070,9 @@
       <c r="Y30">
         <v>1</v>
       </c>
+      <c r="Z30">
+        <v>0</v>
+      </c>
       <c r="AA30">
         <v>15</v>
       </c>
@@ -4082,6 +4169,9 @@
       <c r="Y31">
         <v>0</v>
       </c>
+      <c r="Z31">
+        <v>0</v>
+      </c>
       <c r="AA31">
         <v>15</v>
       </c>
@@ -4178,6 +4268,9 @@
       <c r="Y32">
         <v>1</v>
       </c>
+      <c r="Z32">
+        <v>0</v>
+      </c>
       <c r="AA32">
         <v>16</v>
       </c>
@@ -4274,6 +4367,9 @@
       <c r="Y33">
         <v>1</v>
       </c>
+      <c r="Z33">
+        <v>0</v>
+      </c>
       <c r="AA33">
         <v>17</v>
       </c>
@@ -4370,6 +4466,9 @@
       <c r="Y34">
         <v>0</v>
       </c>
+      <c r="Z34">
+        <v>0</v>
+      </c>
       <c r="AA34">
         <v>16</v>
       </c>
@@ -4466,6 +4565,9 @@
       <c r="Y35">
         <v>0</v>
       </c>
+      <c r="Z35">
+        <v>0</v>
+      </c>
       <c r="AA35">
         <v>17</v>
       </c>
@@ -4562,6 +4664,9 @@
       <c r="Y36">
         <v>1</v>
       </c>
+      <c r="Z36">
+        <v>0</v>
+      </c>
       <c r="AA36">
         <v>18</v>
       </c>
@@ -4658,6 +4763,9 @@
       <c r="Y37">
         <v>0</v>
       </c>
+      <c r="Z37">
+        <v>0</v>
+      </c>
       <c r="AA37">
         <v>18</v>
       </c>
@@ -4754,6 +4862,9 @@
       <c r="Y38">
         <v>1</v>
       </c>
+      <c r="Z38">
+        <v>0</v>
+      </c>
       <c r="AA38">
         <v>19</v>
       </c>
@@ -4850,6 +4961,9 @@
       <c r="Y39">
         <v>0</v>
       </c>
+      <c r="Z39">
+        <v>0</v>
+      </c>
       <c r="AA39">
         <v>19</v>
       </c>
@@ -4946,6 +5060,9 @@
       <c r="Y40">
         <v>0</v>
       </c>
+      <c r="Z40">
+        <v>0</v>
+      </c>
       <c r="AA40">
         <v>20</v>
       </c>
@@ -5042,6 +5159,9 @@
       <c r="Y41">
         <v>1</v>
       </c>
+      <c r="Z41">
+        <v>0</v>
+      </c>
       <c r="AA41">
         <v>20</v>
       </c>
@@ -5138,6 +5258,9 @@
       <c r="Y42">
         <v>1</v>
       </c>
+      <c r="Z42">
+        <v>0</v>
+      </c>
       <c r="AA42">
         <v>21</v>
       </c>
@@ -5234,6 +5357,9 @@
       <c r="Y43">
         <v>0</v>
       </c>
+      <c r="Z43">
+        <v>0</v>
+      </c>
       <c r="AA43">
         <v>21</v>
       </c>
@@ -5330,6 +5456,9 @@
       <c r="Y44">
         <v>0</v>
       </c>
+      <c r="Z44">
+        <v>0</v>
+      </c>
       <c r="AA44">
         <v>22</v>
       </c>
@@ -5426,6 +5555,9 @@
       <c r="Y45">
         <v>1</v>
       </c>
+      <c r="Z45">
+        <v>0</v>
+      </c>
       <c r="AA45">
         <v>22</v>
       </c>
@@ -5522,6 +5654,9 @@
       <c r="Y46">
         <v>1</v>
       </c>
+      <c r="Z46">
+        <v>0</v>
+      </c>
       <c r="AA46">
         <v>23</v>
       </c>
@@ -5618,6 +5753,9 @@
       <c r="Y47">
         <v>0</v>
       </c>
+      <c r="Z47">
+        <v>0</v>
+      </c>
       <c r="AA47">
         <v>23</v>
       </c>
@@ -5714,6 +5852,9 @@
       <c r="Y48">
         <v>1</v>
       </c>
+      <c r="Z48">
+        <v>0</v>
+      </c>
       <c r="AA48">
         <v>24</v>
       </c>
@@ -5810,6 +5951,9 @@
       <c r="Y49">
         <v>0</v>
       </c>
+      <c r="Z49">
+        <v>0</v>
+      </c>
       <c r="AA49">
         <v>24</v>
       </c>
@@ -5906,6 +6050,9 @@
       <c r="Y50">
         <v>1</v>
       </c>
+      <c r="Z50">
+        <v>0</v>
+      </c>
       <c r="AA50">
         <v>25</v>
       </c>
@@ -6002,7 +6149,9 @@
       <c r="Y51" s="5">
         <v>0</v>
       </c>
-      <c r="Z51" s="5"/>
+      <c r="Z51">
+        <v>1</v>
+      </c>
       <c r="AA51" s="5">
         <v>25</v>
       </c>
@@ -6099,6 +6248,9 @@
       <c r="Y52">
         <v>1</v>
       </c>
+      <c r="Z52">
+        <v>0</v>
+      </c>
       <c r="AA52">
         <v>26</v>
       </c>
@@ -6195,6 +6347,9 @@
       <c r="Y53">
         <v>0</v>
       </c>
+      <c r="Z53">
+        <v>0</v>
+      </c>
       <c r="AA53">
         <v>26</v>
       </c>
@@ -6291,7 +6446,9 @@
       <c r="Y54" s="5">
         <v>0</v>
       </c>
-      <c r="Z54" s="5"/>
+      <c r="Z54">
+        <v>0</v>
+      </c>
       <c r="AA54" s="5">
         <v>27</v>
       </c>
@@ -6388,6 +6545,9 @@
       <c r="Y55">
         <v>1</v>
       </c>
+      <c r="Z55">
+        <v>0</v>
+      </c>
       <c r="AA55">
         <v>27</v>
       </c>
@@ -6484,6 +6644,9 @@
       <c r="Y56">
         <v>1</v>
       </c>
+      <c r="Z56">
+        <v>0</v>
+      </c>
       <c r="AA56">
         <v>28</v>
       </c>
@@ -6580,6 +6743,9 @@
       <c r="Y57">
         <v>0</v>
       </c>
+      <c r="Z57">
+        <v>0</v>
+      </c>
       <c r="AA57">
         <v>28</v>
       </c>
@@ -6676,6 +6842,9 @@
       <c r="Y58">
         <v>0</v>
       </c>
+      <c r="Z58">
+        <v>0</v>
+      </c>
       <c r="AA58">
         <v>30</v>
       </c>
@@ -6772,6 +6941,9 @@
       <c r="Y59">
         <v>1</v>
       </c>
+      <c r="Z59">
+        <v>0</v>
+      </c>
       <c r="AA59">
         <v>29</v>
       </c>
@@ -6868,6 +7040,9 @@
       <c r="Y60">
         <v>0</v>
       </c>
+      <c r="Z60">
+        <v>0</v>
+      </c>
       <c r="AA60">
         <v>29</v>
       </c>
@@ -6964,6 +7139,9 @@
       <c r="Y61">
         <v>1</v>
       </c>
+      <c r="Z61">
+        <v>0</v>
+      </c>
       <c r="AA61">
         <v>30</v>
       </c>
@@ -7060,6 +7238,9 @@
       <c r="Y62">
         <v>1</v>
       </c>
+      <c r="Z62">
+        <v>0</v>
+      </c>
       <c r="AA62">
         <v>31</v>
       </c>
@@ -7156,6 +7337,9 @@
       <c r="Y63">
         <v>0</v>
       </c>
+      <c r="Z63">
+        <v>0</v>
+      </c>
       <c r="AA63">
         <v>32</v>
       </c>
@@ -7252,6 +7436,9 @@
       <c r="Y64">
         <v>1</v>
       </c>
+      <c r="Z64">
+        <v>0</v>
+      </c>
       <c r="AA64">
         <v>32</v>
       </c>
@@ -7348,6 +7535,9 @@
       <c r="Y65">
         <v>0</v>
       </c>
+      <c r="Z65">
+        <v>0</v>
+      </c>
       <c r="AA65">
         <v>31</v>
       </c>
@@ -7444,6 +7634,9 @@
       <c r="Y66">
         <v>1</v>
       </c>
+      <c r="Z66">
+        <v>0</v>
+      </c>
       <c r="AA66">
         <v>33</v>
       </c>
@@ -7540,6 +7733,9 @@
       <c r="Y67">
         <v>0</v>
       </c>
+      <c r="Z67">
+        <v>0</v>
+      </c>
       <c r="AA67">
         <v>33</v>
       </c>
@@ -7636,6 +7832,9 @@
       <c r="Y68">
         <v>1</v>
       </c>
+      <c r="Z68">
+        <v>0</v>
+      </c>
       <c r="AA68">
         <v>34</v>
       </c>
@@ -7732,6 +7931,9 @@
       <c r="Y69">
         <v>0</v>
       </c>
+      <c r="Z69">
+        <v>0</v>
+      </c>
       <c r="AA69">
         <v>34</v>
       </c>
@@ -7828,6 +8030,9 @@
       <c r="Y70">
         <v>1</v>
       </c>
+      <c r="Z70">
+        <v>0</v>
+      </c>
       <c r="AA70">
         <v>35</v>
       </c>
@@ -7924,6 +8129,9 @@
       <c r="Y71">
         <v>0</v>
       </c>
+      <c r="Z71">
+        <v>0</v>
+      </c>
       <c r="AA71">
         <v>35</v>
       </c>
@@ -8020,6 +8228,9 @@
       <c r="Y72">
         <v>1</v>
       </c>
+      <c r="Z72">
+        <v>0</v>
+      </c>
       <c r="AA72">
         <v>36</v>
       </c>
@@ -8116,6 +8327,9 @@
       <c r="Y73">
         <v>0</v>
       </c>
+      <c r="Z73">
+        <v>0</v>
+      </c>
       <c r="AA73">
         <v>36</v>
       </c>
@@ -8212,6 +8426,9 @@
       <c r="Y74">
         <v>0</v>
       </c>
+      <c r="Z74">
+        <v>0</v>
+      </c>
       <c r="AA74">
         <v>37</v>
       </c>
@@ -8308,6 +8525,9 @@
       <c r="Y75">
         <v>0</v>
       </c>
+      <c r="Z75">
+        <v>0</v>
+      </c>
       <c r="AA75">
         <v>38</v>
       </c>
@@ -8404,6 +8624,9 @@
       <c r="Y76">
         <v>1</v>
       </c>
+      <c r="Z76">
+        <v>1</v>
+      </c>
       <c r="AA76">
         <v>37</v>
       </c>
@@ -8500,6 +8723,9 @@
       <c r="Y77">
         <v>0</v>
       </c>
+      <c r="Z77">
+        <v>0</v>
+      </c>
       <c r="AA77">
         <v>39</v>
       </c>
@@ -8596,6 +8822,9 @@
       <c r="Y78">
         <v>1</v>
       </c>
+      <c r="Z78">
+        <v>0</v>
+      </c>
       <c r="AA78">
         <v>38</v>
       </c>
@@ -8692,6 +8921,9 @@
       <c r="Y79">
         <v>1</v>
       </c>
+      <c r="Z79">
+        <v>0</v>
+      </c>
       <c r="AA79">
         <v>39</v>
       </c>
@@ -8788,6 +9020,9 @@
       <c r="Y80">
         <v>0</v>
       </c>
+      <c r="Z80">
+        <v>0</v>
+      </c>
       <c r="AA80">
         <v>40</v>
       </c>
@@ -8884,6 +9119,9 @@
       <c r="Y81">
         <v>0</v>
       </c>
+      <c r="Z81">
+        <v>0</v>
+      </c>
       <c r="AA81">
         <v>42</v>
       </c>
@@ -8980,6 +9218,9 @@
       <c r="Y82">
         <v>1</v>
       </c>
+      <c r="Z82">
+        <v>0</v>
+      </c>
       <c r="AA82">
         <v>40</v>
       </c>
@@ -9076,6 +9317,9 @@
       <c r="Y83">
         <v>1</v>
       </c>
+      <c r="Z83">
+        <v>0</v>
+      </c>
       <c r="AA83">
         <v>41</v>
       </c>
@@ -9172,6 +9416,9 @@
       <c r="Y84">
         <v>0</v>
       </c>
+      <c r="Z84">
+        <v>0</v>
+      </c>
       <c r="AA84">
         <v>41</v>
       </c>
@@ -9268,6 +9515,9 @@
       <c r="Y85">
         <v>1</v>
       </c>
+      <c r="Z85">
+        <v>0</v>
+      </c>
       <c r="AA85">
         <v>42</v>
       </c>
@@ -9364,6 +9614,9 @@
       <c r="Y86">
         <v>0</v>
       </c>
+      <c r="Z86">
+        <v>0</v>
+      </c>
       <c r="AA86">
         <v>43</v>
       </c>
@@ -9460,6 +9713,9 @@
       <c r="Y87">
         <v>1</v>
       </c>
+      <c r="Z87">
+        <v>0</v>
+      </c>
       <c r="AA87">
         <v>43</v>
       </c>
@@ -9556,6 +9812,9 @@
       <c r="Y88">
         <v>0</v>
       </c>
+      <c r="Z88">
+        <v>0</v>
+      </c>
       <c r="AA88">
         <v>44</v>
       </c>
@@ -9652,6 +9911,9 @@
       <c r="Y89">
         <v>1</v>
       </c>
+      <c r="Z89">
+        <v>0</v>
+      </c>
       <c r="AA89">
         <v>44</v>
       </c>
@@ -9748,6 +10010,9 @@
       <c r="Y90">
         <v>0</v>
       </c>
+      <c r="Z90">
+        <v>0</v>
+      </c>
       <c r="AA90">
         <v>45</v>
       </c>
@@ -9844,6 +10109,9 @@
       <c r="Y91">
         <v>1</v>
       </c>
+      <c r="Z91">
+        <v>0</v>
+      </c>
       <c r="AA91">
         <v>45</v>
       </c>
@@ -9940,6 +10208,9 @@
       <c r="Y92">
         <v>1</v>
       </c>
+      <c r="Z92">
+        <v>0</v>
+      </c>
       <c r="AA92">
         <v>46</v>
       </c>
@@ -10036,6 +10307,9 @@
       <c r="Y93">
         <v>0</v>
       </c>
+      <c r="Z93">
+        <v>0</v>
+      </c>
       <c r="AA93">
         <v>46</v>
       </c>
@@ -10132,7 +10406,9 @@
       <c r="Y94" s="5">
         <v>0</v>
       </c>
-      <c r="Z94" s="5"/>
+      <c r="Z94">
+        <v>0</v>
+      </c>
       <c r="AA94" s="5">
         <v>47</v>
       </c>
@@ -10229,7 +10505,9 @@
       <c r="Y95" s="5">
         <v>0</v>
       </c>
-      <c r="Z95" s="5"/>
+      <c r="Z95">
+        <v>0</v>
+      </c>
       <c r="AA95" s="5">
         <v>48</v>
       </c>
@@ -10326,6 +10604,9 @@
       <c r="Y96">
         <v>1</v>
       </c>
+      <c r="Z96">
+        <v>0</v>
+      </c>
       <c r="AA96">
         <v>47</v>
       </c>
@@ -10422,6 +10703,9 @@
       <c r="Y97">
         <v>1</v>
       </c>
+      <c r="Z97">
+        <v>0</v>
+      </c>
       <c r="AA97">
         <v>48</v>
       </c>
@@ -10490,7 +10774,7 @@
         <v>14</v>
       </c>
       <c r="R98">
-        <f t="shared" ref="R98:R129" si="34">IF(L98=0,P98,Q98)</f>
+        <f t="shared" ref="R98:R109" si="34">IF(L98=0,P98,Q98)</f>
         <v>14</v>
       </c>
       <c r="S98">
@@ -10518,6 +10802,9 @@
       <c r="Y98">
         <v>0</v>
       </c>
+      <c r="Z98">
+        <v>0</v>
+      </c>
       <c r="AA98">
         <v>49</v>
       </c>
@@ -10614,6 +10901,9 @@
       <c r="Y99">
         <v>0</v>
       </c>
+      <c r="Z99">
+        <v>0</v>
+      </c>
       <c r="AA99">
         <v>50</v>
       </c>
@@ -10710,6 +11000,9 @@
       <c r="Y100">
         <v>1</v>
       </c>
+      <c r="Z100">
+        <v>0</v>
+      </c>
       <c r="AA100">
         <v>49</v>
       </c>
@@ -10806,6 +11099,9 @@
       <c r="Y101">
         <v>0</v>
       </c>
+      <c r="Z101">
+        <v>1</v>
+      </c>
       <c r="AA101">
         <v>51</v>
       </c>
@@ -10902,6 +11198,9 @@
       <c r="Y102">
         <v>1</v>
       </c>
+      <c r="Z102">
+        <v>0</v>
+      </c>
       <c r="AA102">
         <v>50</v>
       </c>
@@ -10998,6 +11297,9 @@
       <c r="Y103">
         <v>1</v>
       </c>
+      <c r="Z103">
+        <v>0</v>
+      </c>
       <c r="AA103">
         <v>51</v>
       </c>
@@ -11094,6 +11396,9 @@
       <c r="Y104">
         <v>0</v>
       </c>
+      <c r="Z104">
+        <v>0</v>
+      </c>
       <c r="AA104">
         <v>52</v>
       </c>
@@ -11190,6 +11495,9 @@
       <c r="Y105">
         <v>0</v>
       </c>
+      <c r="Z105">
+        <v>0</v>
+      </c>
       <c r="AA105">
         <v>53</v>
       </c>
@@ -11286,6 +11594,9 @@
       <c r="Y106">
         <v>1</v>
       </c>
+      <c r="Z106">
+        <v>0</v>
+      </c>
       <c r="AA106">
         <v>52</v>
       </c>
@@ -11382,6 +11693,9 @@
       <c r="Y107">
         <v>0</v>
       </c>
+      <c r="Z107">
+        <v>0</v>
+      </c>
       <c r="AA107">
         <v>54</v>
       </c>
@@ -11478,6 +11792,9 @@
       <c r="Y108">
         <v>1</v>
       </c>
+      <c r="Z108">
+        <v>0</v>
+      </c>
       <c r="AA108">
         <v>53</v>
       </c>
@@ -11574,6 +11891,9 @@
       <c r="Y109">
         <v>1</v>
       </c>
+      <c r="Z109">
+        <v>0</v>
+      </c>
       <c r="AA109">
         <v>54</v>
       </c>
@@ -11583,6 +11903,36 @@
       </c>
       <c r="AC109">
         <v>18</v>
+      </c>
+    </row>
+    <row r="110" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="Z110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="Z111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="Z112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="26:26" x14ac:dyDescent="0.2">
+      <c r="Z113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="26:26" x14ac:dyDescent="0.2">
+      <c r="Z114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="26:26" x14ac:dyDescent="0.2">
+      <c r="Z115">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor: set unused and incorrect 'probviol' learn list column to NaN
</commit_message>
<xml_diff>
--- a/lists/learn_list_study4_base.xlsx
+++ b/lists/learn_list_study4_base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gelliott/Documents/projects/delaylearn/feedback-delay-four/lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5F6A3B-F0BE-C641-96F1-F5227638F261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B4F3CB-A02C-9C45-9357-2AEDA0F77013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="1240" windowWidth="43380" windowHeight="27560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="list_study4_try_counter1" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="64">
   <si>
     <t>pattern_stimuli</t>
   </si>
@@ -1143,7 +1143,7 @@
   <dimension ref="A1:AF109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K109"/>
+      <selection activeCell="J2" sqref="J2:J109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1288,8 +1288,8 @@
         <f t="shared" ref="I2:I33" si="3">IF(AND(Y2=1,O2=0),"f",IF(AND(Y2=1,O2=1),"j",IF(AND(Y2=0,O2=0),"j","f")))</f>
         <v>f</v>
       </c>
-      <c r="J2">
-        <v>0</v>
+      <c r="J2" t="s">
+        <v>63</v>
       </c>
       <c r="K2" t="s">
         <v>63</v>
@@ -1395,8 +1395,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J3">
-        <v>0</v>
+      <c r="J3" t="s">
+        <v>63</v>
       </c>
       <c r="K3" t="s">
         <v>63</v>
@@ -1502,8 +1502,8 @@
         <f t="shared" si="3"/>
         <v>f</v>
       </c>
-      <c r="J4">
-        <v>0</v>
+      <c r="J4" t="s">
+        <v>63</v>
       </c>
       <c r="K4" t="s">
         <v>63</v>
@@ -1611,8 +1611,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J5">
-        <v>0</v>
+      <c r="J5" t="s">
+        <v>63</v>
       </c>
       <c r="K5" t="s">
         <v>63</v>
@@ -1720,8 +1720,8 @@
         <f t="shared" si="3"/>
         <v>f</v>
       </c>
-      <c r="J6" s="6">
-        <v>1</v>
+      <c r="J6" t="s">
+        <v>63</v>
       </c>
       <c r="K6" t="s">
         <v>63</v>
@@ -1829,8 +1829,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J7">
-        <v>0</v>
+      <c r="J7" t="s">
+        <v>63</v>
       </c>
       <c r="K7" t="s">
         <v>63</v>
@@ -1938,8 +1938,8 @@
         <f t="shared" si="3"/>
         <v>f</v>
       </c>
-      <c r="J8">
-        <v>1</v>
+      <c r="J8" t="s">
+        <v>63</v>
       </c>
       <c r="K8" t="s">
         <v>63</v>
@@ -2047,8 +2047,8 @@
         <f t="shared" si="3"/>
         <v>f</v>
       </c>
-      <c r="J9">
-        <v>0</v>
+      <c r="J9" t="s">
+        <v>63</v>
       </c>
       <c r="K9" t="s">
         <v>63</v>
@@ -2156,8 +2156,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J10" s="6">
-        <v>0</v>
+      <c r="J10" t="s">
+        <v>63</v>
       </c>
       <c r="K10" t="s">
         <v>63</v>
@@ -2265,8 +2265,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J11">
-        <v>0</v>
+      <c r="J11" t="s">
+        <v>63</v>
       </c>
       <c r="K11" t="s">
         <v>63</v>
@@ -2374,8 +2374,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J12">
-        <v>0</v>
+      <c r="J12" t="s">
+        <v>63</v>
       </c>
       <c r="K12" t="s">
         <v>63</v>
@@ -2483,8 +2483,8 @@
         <f t="shared" si="3"/>
         <v>f</v>
       </c>
-      <c r="J13">
-        <v>0</v>
+      <c r="J13" t="s">
+        <v>63</v>
       </c>
       <c r="K13" t="s">
         <v>63</v>
@@ -2592,8 +2592,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J14">
-        <v>0</v>
+      <c r="J14" t="s">
+        <v>63</v>
       </c>
       <c r="K14" t="s">
         <v>63</v>
@@ -2701,8 +2701,8 @@
         <f t="shared" si="3"/>
         <v>f</v>
       </c>
-      <c r="J15">
-        <v>0</v>
+      <c r="J15" t="s">
+        <v>63</v>
       </c>
       <c r="K15" t="s">
         <v>63</v>
@@ -2810,8 +2810,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J16">
-        <v>0</v>
+      <c r="J16" t="s">
+        <v>63</v>
       </c>
       <c r="K16" t="s">
         <v>63</v>
@@ -2919,8 +2919,8 @@
         <f t="shared" si="3"/>
         <v>f</v>
       </c>
-      <c r="J17">
-        <v>1</v>
+      <c r="J17" t="s">
+        <v>63</v>
       </c>
       <c r="K17" t="s">
         <v>63</v>
@@ -3028,8 +3028,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J18">
-        <v>0</v>
+      <c r="J18" t="s">
+        <v>63</v>
       </c>
       <c r="K18" t="s">
         <v>63</v>
@@ -3137,8 +3137,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J19">
-        <v>0</v>
+      <c r="J19" t="s">
+        <v>63</v>
       </c>
       <c r="K19" t="s">
         <v>63</v>
@@ -3246,8 +3246,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J20">
-        <v>0</v>
+      <c r="J20" t="s">
+        <v>63</v>
       </c>
       <c r="K20" t="s">
         <v>63</v>
@@ -3355,8 +3355,8 @@
         <f t="shared" si="3"/>
         <v>f</v>
       </c>
-      <c r="J21">
-        <v>0</v>
+      <c r="J21" t="s">
+        <v>63</v>
       </c>
       <c r="K21" t="s">
         <v>63</v>
@@ -3464,8 +3464,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J22">
-        <v>0</v>
+      <c r="J22" t="s">
+        <v>63</v>
       </c>
       <c r="K22" t="s">
         <v>63</v>
@@ -3573,8 +3573,8 @@
         <f t="shared" si="3"/>
         <v>f</v>
       </c>
-      <c r="J23">
-        <v>1</v>
+      <c r="J23" t="s">
+        <v>63</v>
       </c>
       <c r="K23" t="s">
         <v>63</v>
@@ -3682,8 +3682,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J24">
-        <v>0</v>
+      <c r="J24" t="s">
+        <v>63</v>
       </c>
       <c r="K24" t="s">
         <v>63</v>
@@ -3791,8 +3791,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J25">
-        <v>0</v>
+      <c r="J25" t="s">
+        <v>63</v>
       </c>
       <c r="K25" t="s">
         <v>63</v>
@@ -3900,8 +3900,8 @@
         <f t="shared" si="3"/>
         <v>f</v>
       </c>
-      <c r="J26">
-        <v>0</v>
+      <c r="J26" t="s">
+        <v>63</v>
       </c>
       <c r="K26" t="s">
         <v>63</v>
@@ -4009,8 +4009,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J27">
-        <v>0</v>
+      <c r="J27" t="s">
+        <v>63</v>
       </c>
       <c r="K27" t="s">
         <v>63</v>
@@ -4118,8 +4118,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J28">
-        <v>0</v>
+      <c r="J28" t="s">
+        <v>63</v>
       </c>
       <c r="K28" t="s">
         <v>63</v>
@@ -4227,8 +4227,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J29">
-        <v>0</v>
+      <c r="J29" t="s">
+        <v>63</v>
       </c>
       <c r="K29" t="s">
         <v>63</v>
@@ -4336,8 +4336,8 @@
         <f t="shared" si="3"/>
         <v>f</v>
       </c>
-      <c r="J30">
-        <v>1</v>
+      <c r="J30" t="s">
+        <v>63</v>
       </c>
       <c r="K30" t="s">
         <v>63</v>
@@ -4445,8 +4445,8 @@
         <f t="shared" si="3"/>
         <v>f</v>
       </c>
-      <c r="J31">
-        <v>1</v>
+      <c r="J31" t="s">
+        <v>63</v>
       </c>
       <c r="K31" t="s">
         <v>63</v>
@@ -4554,8 +4554,8 @@
         <f t="shared" si="3"/>
         <v>f</v>
       </c>
-      <c r="J32">
-        <v>0</v>
+      <c r="J32" t="s">
+        <v>63</v>
       </c>
       <c r="K32" t="s">
         <v>63</v>
@@ -4663,8 +4663,8 @@
         <f t="shared" si="3"/>
         <v>j</v>
       </c>
-      <c r="J33">
-        <v>1</v>
+      <c r="J33" t="s">
+        <v>63</v>
       </c>
       <c r="K33" t="s">
         <v>63</v>
@@ -4772,8 +4772,8 @@
         <f t="shared" ref="I34:I65" si="14">IF(AND(Y34=1,O34=0),"f",IF(AND(Y34=1,O34=1),"j",IF(AND(Y34=0,O34=0),"j","f")))</f>
         <v>j</v>
       </c>
-      <c r="J34">
-        <v>0</v>
+      <c r="J34" t="s">
+        <v>63</v>
       </c>
       <c r="K34" t="s">
         <v>63</v>
@@ -4881,8 +4881,8 @@
         <f t="shared" si="14"/>
         <v>j</v>
       </c>
-      <c r="J35">
-        <v>0</v>
+      <c r="J35" t="s">
+        <v>63</v>
       </c>
       <c r="K35" t="s">
         <v>63</v>
@@ -4990,8 +4990,8 @@
         <f t="shared" si="14"/>
         <v>f</v>
       </c>
-      <c r="J36">
-        <v>0</v>
+      <c r="J36" t="s">
+        <v>63</v>
       </c>
       <c r="K36" t="s">
         <v>63</v>
@@ -5099,8 +5099,8 @@
         <f t="shared" si="14"/>
         <v>j</v>
       </c>
-      <c r="J37">
-        <v>1</v>
+      <c r="J37" t="s">
+        <v>63</v>
       </c>
       <c r="K37" t="s">
         <v>63</v>
@@ -5208,8 +5208,8 @@
         <f t="shared" si="14"/>
         <v>j</v>
       </c>
-      <c r="J38">
-        <v>0</v>
+      <c r="J38" t="s">
+        <v>63</v>
       </c>
       <c r="K38" t="s">
         <v>63</v>
@@ -5317,8 +5317,8 @@
         <f t="shared" si="14"/>
         <v>f</v>
       </c>
-      <c r="J39">
-        <v>1</v>
+      <c r="J39" t="s">
+        <v>63</v>
       </c>
       <c r="K39" t="s">
         <v>63</v>
@@ -5426,8 +5426,8 @@
         <f t="shared" si="14"/>
         <v>f</v>
       </c>
-      <c r="J40">
-        <v>0</v>
+      <c r="J40" t="s">
+        <v>63</v>
       </c>
       <c r="K40" t="s">
         <v>63</v>
@@ -5535,8 +5535,8 @@
         <f t="shared" si="14"/>
         <v>f</v>
       </c>
-      <c r="J41">
-        <v>1</v>
+      <c r="J41" t="s">
+        <v>63</v>
       </c>
       <c r="K41" t="s">
         <v>63</v>
@@ -5644,8 +5644,8 @@
         <f t="shared" si="14"/>
         <v>j</v>
       </c>
-      <c r="J42">
-        <v>0</v>
+      <c r="J42" t="s">
+        <v>63</v>
       </c>
       <c r="K42" t="s">
         <v>63</v>
@@ -5753,8 +5753,8 @@
         <f t="shared" si="14"/>
         <v>j</v>
       </c>
-      <c r="J43">
-        <v>0</v>
+      <c r="J43" t="s">
+        <v>63</v>
       </c>
       <c r="K43" t="s">
         <v>63</v>
@@ -5862,8 +5862,8 @@
         <f t="shared" si="14"/>
         <v>f</v>
       </c>
-      <c r="J44">
-        <v>0</v>
+      <c r="J44" t="s">
+        <v>63</v>
       </c>
       <c r="K44" t="s">
         <v>63</v>
@@ -5971,8 +5971,8 @@
         <f t="shared" si="14"/>
         <v>f</v>
       </c>
-      <c r="J45">
-        <v>0</v>
+      <c r="J45" t="s">
+        <v>63</v>
       </c>
       <c r="K45" t="s">
         <v>63</v>
@@ -6080,8 +6080,8 @@
         <f t="shared" si="14"/>
         <v>f</v>
       </c>
-      <c r="J46">
-        <v>0</v>
+      <c r="J46" t="s">
+        <v>63</v>
       </c>
       <c r="K46" t="s">
         <v>63</v>
@@ -6189,8 +6189,8 @@
         <f t="shared" si="14"/>
         <v>j</v>
       </c>
-      <c r="J47">
-        <v>0</v>
+      <c r="J47" t="s">
+        <v>63</v>
       </c>
       <c r="K47" t="s">
         <v>63</v>
@@ -6298,8 +6298,8 @@
         <f t="shared" si="14"/>
         <v>j</v>
       </c>
-      <c r="J48">
-        <v>1</v>
+      <c r="J48" t="s">
+        <v>63</v>
       </c>
       <c r="K48" t="s">
         <v>63</v>
@@ -6407,8 +6407,8 @@
         <f t="shared" si="14"/>
         <v>f</v>
       </c>
-      <c r="J49">
-        <v>0</v>
+      <c r="J49" t="s">
+        <v>63</v>
       </c>
       <c r="K49" t="s">
         <v>63</v>
@@ -6516,8 +6516,8 @@
         <f t="shared" si="14"/>
         <v>f</v>
       </c>
-      <c r="J50">
-        <v>0</v>
+      <c r="J50" t="s">
+        <v>63</v>
       </c>
       <c r="K50" t="s">
         <v>63</v>
@@ -6625,8 +6625,8 @@
         <f t="shared" si="14"/>
         <v>j</v>
       </c>
-      <c r="J51">
-        <v>0</v>
+      <c r="J51" t="s">
+        <v>63</v>
       </c>
       <c r="K51" t="s">
         <v>63</v>
@@ -6734,8 +6734,8 @@
         <f t="shared" si="14"/>
         <v>j</v>
       </c>
-      <c r="J52">
-        <v>0</v>
+      <c r="J52" t="s">
+        <v>63</v>
       </c>
       <c r="K52" t="s">
         <v>63</v>
@@ -6843,8 +6843,8 @@
         <f t="shared" si="14"/>
         <v>j</v>
       </c>
-      <c r="J53">
-        <v>0</v>
+      <c r="J53" t="s">
+        <v>63</v>
       </c>
       <c r="K53" t="s">
         <v>63</v>
@@ -6952,8 +6952,8 @@
         <f t="shared" si="14"/>
         <v>f</v>
       </c>
-      <c r="J54">
-        <v>1</v>
+      <c r="J54" t="s">
+        <v>63</v>
       </c>
       <c r="K54" t="s">
         <v>63</v>
@@ -7061,8 +7061,8 @@
         <f t="shared" si="14"/>
         <v>f</v>
       </c>
-      <c r="J55">
-        <v>0</v>
+      <c r="J55" t="s">
+        <v>63</v>
       </c>
       <c r="K55" t="s">
         <v>63</v>
@@ -7170,8 +7170,8 @@
         <f t="shared" si="14"/>
         <v>j</v>
       </c>
-      <c r="J56">
-        <v>0</v>
+      <c r="J56" t="s">
+        <v>63</v>
       </c>
       <c r="K56" t="s">
         <v>63</v>
@@ -7279,8 +7279,8 @@
         <f t="shared" si="14"/>
         <v>j</v>
       </c>
-      <c r="J57">
-        <v>1</v>
+      <c r="J57" t="s">
+        <v>63</v>
       </c>
       <c r="K57" t="s">
         <v>63</v>
@@ -7388,8 +7388,8 @@
         <f t="shared" si="14"/>
         <v>f</v>
       </c>
-      <c r="J58">
-        <v>0</v>
+      <c r="J58" t="s">
+        <v>63</v>
       </c>
       <c r="K58" t="s">
         <v>63</v>
@@ -7497,8 +7497,8 @@
         <f t="shared" si="14"/>
         <v>j</v>
       </c>
-      <c r="J59">
-        <v>0</v>
+      <c r="J59" t="s">
+        <v>63</v>
       </c>
       <c r="K59" t="s">
         <v>63</v>
@@ -7606,8 +7606,8 @@
         <f t="shared" si="14"/>
         <v>j</v>
       </c>
-      <c r="J60">
-        <v>0</v>
+      <c r="J60" t="s">
+        <v>63</v>
       </c>
       <c r="K60" t="s">
         <v>63</v>
@@ -7715,8 +7715,8 @@
         <f t="shared" si="14"/>
         <v>f</v>
       </c>
-      <c r="J61">
-        <v>0</v>
+      <c r="J61" t="s">
+        <v>63</v>
       </c>
       <c r="K61" t="s">
         <v>63</v>
@@ -7824,8 +7824,8 @@
         <f t="shared" si="14"/>
         <v>f</v>
       </c>
-      <c r="J62">
-        <v>0</v>
+      <c r="J62" t="s">
+        <v>63</v>
       </c>
       <c r="K62" t="s">
         <v>63</v>
@@ -7933,8 +7933,8 @@
         <f t="shared" si="14"/>
         <v>f</v>
       </c>
-      <c r="J63">
-        <v>0</v>
+      <c r="J63" t="s">
+        <v>63</v>
       </c>
       <c r="K63" t="s">
         <v>63</v>
@@ -8042,8 +8042,8 @@
         <f t="shared" si="14"/>
         <v>j</v>
       </c>
-      <c r="J64">
-        <v>0</v>
+      <c r="J64" t="s">
+        <v>63</v>
       </c>
       <c r="K64" t="s">
         <v>63</v>
@@ -8151,8 +8151,8 @@
         <f t="shared" si="14"/>
         <v>f</v>
       </c>
-      <c r="J65">
-        <v>0</v>
+      <c r="J65" t="s">
+        <v>63</v>
       </c>
       <c r="K65" t="s">
         <v>63</v>
@@ -8260,8 +8260,8 @@
         <f t="shared" ref="I66:I97" si="25">IF(AND(Y66=1,O66=0),"f",IF(AND(Y66=1,O66=1),"j",IF(AND(Y66=0,O66=0),"j","f")))</f>
         <v>j</v>
       </c>
-      <c r="J66">
-        <v>1</v>
+      <c r="J66" t="s">
+        <v>63</v>
       </c>
       <c r="K66" t="s">
         <v>63</v>
@@ -8369,8 +8369,8 @@
         <f t="shared" si="25"/>
         <v>f</v>
       </c>
-      <c r="J67">
-        <v>0</v>
+      <c r="J67" t="s">
+        <v>63</v>
       </c>
       <c r="K67" t="s">
         <v>63</v>
@@ -8478,8 +8478,8 @@
         <f t="shared" si="25"/>
         <v>j</v>
       </c>
-      <c r="J68">
-        <v>0</v>
+      <c r="J68" t="s">
+        <v>63</v>
       </c>
       <c r="K68" t="s">
         <v>63</v>
@@ -8587,8 +8587,8 @@
         <f t="shared" si="25"/>
         <v>f</v>
       </c>
-      <c r="J69">
-        <v>1</v>
+      <c r="J69" t="s">
+        <v>63</v>
       </c>
       <c r="K69" t="s">
         <v>63</v>
@@ -8696,8 +8696,8 @@
         <f t="shared" si="25"/>
         <v>j</v>
       </c>
-      <c r="J70">
-        <v>0</v>
+      <c r="J70" t="s">
+        <v>63</v>
       </c>
       <c r="K70" t="s">
         <v>63</v>
@@ -8805,8 +8805,8 @@
         <f t="shared" si="25"/>
         <v>f</v>
       </c>
-      <c r="J71">
-        <v>0</v>
+      <c r="J71" t="s">
+        <v>63</v>
       </c>
       <c r="K71" t="s">
         <v>63</v>
@@ -8914,8 +8914,8 @@
         <f t="shared" si="25"/>
         <v>j</v>
       </c>
-      <c r="J72">
-        <v>1</v>
+      <c r="J72" t="s">
+        <v>63</v>
       </c>
       <c r="K72" t="s">
         <v>63</v>
@@ -9023,8 +9023,8 @@
         <f t="shared" si="25"/>
         <v>j</v>
       </c>
-      <c r="J73">
-        <v>1</v>
+      <c r="J73" t="s">
+        <v>63</v>
       </c>
       <c r="K73" t="s">
         <v>63</v>
@@ -9132,8 +9132,8 @@
         <f t="shared" si="25"/>
         <v>j</v>
       </c>
-      <c r="J74">
-        <v>0</v>
+      <c r="J74" t="s">
+        <v>63</v>
       </c>
       <c r="K74" t="s">
         <v>63</v>
@@ -9241,8 +9241,8 @@
         <f t="shared" si="25"/>
         <v>j</v>
       </c>
-      <c r="J75">
-        <v>0</v>
+      <c r="J75" t="s">
+        <v>63</v>
       </c>
       <c r="K75" t="s">
         <v>63</v>
@@ -9350,8 +9350,8 @@
         <f t="shared" si="25"/>
         <v>j</v>
       </c>
-      <c r="J76">
-        <v>0</v>
+      <c r="J76" t="s">
+        <v>63</v>
       </c>
       <c r="K76" t="s">
         <v>63</v>
@@ -9459,8 +9459,8 @@
         <f t="shared" si="25"/>
         <v>f</v>
       </c>
-      <c r="J77">
-        <v>0</v>
+      <c r="J77" t="s">
+        <v>63</v>
       </c>
       <c r="K77" t="s">
         <v>63</v>
@@ -9568,8 +9568,8 @@
         <f t="shared" si="25"/>
         <v>f</v>
       </c>
-      <c r="J78">
-        <v>0</v>
+      <c r="J78" t="s">
+        <v>63</v>
       </c>
       <c r="K78" t="s">
         <v>63</v>
@@ -9677,8 +9677,8 @@
         <f t="shared" si="25"/>
         <v>f</v>
       </c>
-      <c r="J79">
-        <v>0</v>
+      <c r="J79" t="s">
+        <v>63</v>
       </c>
       <c r="K79" t="s">
         <v>63</v>
@@ -9786,8 +9786,8 @@
         <f t="shared" si="25"/>
         <v>f</v>
       </c>
-      <c r="J80">
-        <v>0</v>
+      <c r="J80" t="s">
+        <v>63</v>
       </c>
       <c r="K80" t="s">
         <v>63</v>
@@ -9895,8 +9895,8 @@
         <f t="shared" si="25"/>
         <v>f</v>
       </c>
-      <c r="J81">
-        <v>0</v>
+      <c r="J81" t="s">
+        <v>63</v>
       </c>
       <c r="K81" t="s">
         <v>63</v>
@@ -10004,8 +10004,8 @@
         <f t="shared" si="25"/>
         <v>f</v>
       </c>
-      <c r="J82">
-        <v>0</v>
+      <c r="J82" t="s">
+        <v>63</v>
       </c>
       <c r="K82" t="s">
         <v>63</v>
@@ -10113,8 +10113,8 @@
         <f t="shared" si="25"/>
         <v>f</v>
       </c>
-      <c r="J83">
-        <v>0</v>
+      <c r="J83" t="s">
+        <v>63</v>
       </c>
       <c r="K83" t="s">
         <v>63</v>
@@ -10222,8 +10222,8 @@
         <f t="shared" si="25"/>
         <v>j</v>
       </c>
-      <c r="J84">
-        <v>1</v>
+      <c r="J84" t="s">
+        <v>63</v>
       </c>
       <c r="K84" t="s">
         <v>63</v>
@@ -10331,8 +10331,8 @@
         <f t="shared" si="25"/>
         <v>f</v>
       </c>
-      <c r="J85">
-        <v>1</v>
+      <c r="J85" t="s">
+        <v>63</v>
       </c>
       <c r="K85" t="s">
         <v>63</v>
@@ -10440,8 +10440,8 @@
         <f t="shared" si="25"/>
         <v>f</v>
       </c>
-      <c r="J86">
-        <v>1</v>
+      <c r="J86" t="s">
+        <v>63</v>
       </c>
       <c r="K86" t="s">
         <v>63</v>
@@ -10549,8 +10549,8 @@
         <f t="shared" si="25"/>
         <v>j</v>
       </c>
-      <c r="J87">
-        <v>0</v>
+      <c r="J87" t="s">
+        <v>63</v>
       </c>
       <c r="K87" t="s">
         <v>63</v>
@@ -10658,8 +10658,8 @@
         <f t="shared" si="25"/>
         <v>f</v>
       </c>
-      <c r="J88">
-        <v>0</v>
+      <c r="J88" t="s">
+        <v>63</v>
       </c>
       <c r="K88" t="s">
         <v>63</v>
@@ -10767,8 +10767,8 @@
         <f t="shared" si="25"/>
         <v>f</v>
       </c>
-      <c r="J89">
-        <v>0</v>
+      <c r="J89" t="s">
+        <v>63</v>
       </c>
       <c r="K89" t="s">
         <v>63</v>
@@ -10876,8 +10876,8 @@
         <f t="shared" si="25"/>
         <v>j</v>
       </c>
-      <c r="J90">
-        <v>0</v>
+      <c r="J90" t="s">
+        <v>63</v>
       </c>
       <c r="K90" t="s">
         <v>63</v>
@@ -10985,8 +10985,8 @@
         <f t="shared" si="25"/>
         <v>j</v>
       </c>
-      <c r="J91">
-        <v>1</v>
+      <c r="J91" t="s">
+        <v>63</v>
       </c>
       <c r="K91" t="s">
         <v>63</v>
@@ -11094,8 +11094,8 @@
         <f t="shared" si="25"/>
         <v>f</v>
       </c>
-      <c r="J92">
-        <v>0</v>
+      <c r="J92" t="s">
+        <v>63</v>
       </c>
       <c r="K92" t="s">
         <v>63</v>
@@ -11203,8 +11203,8 @@
         <f t="shared" si="25"/>
         <v>j</v>
       </c>
-      <c r="J93">
-        <v>0</v>
+      <c r="J93" t="s">
+        <v>63</v>
       </c>
       <c r="K93" t="s">
         <v>63</v>
@@ -11312,8 +11312,8 @@
         <f t="shared" si="25"/>
         <v>j</v>
       </c>
-      <c r="J94">
-        <v>0</v>
+      <c r="J94" t="s">
+        <v>63</v>
       </c>
       <c r="K94" t="s">
         <v>63</v>
@@ -11421,8 +11421,8 @@
         <f t="shared" si="25"/>
         <v>f</v>
       </c>
-      <c r="J95">
-        <v>0</v>
+      <c r="J95" t="s">
+        <v>63</v>
       </c>
       <c r="K95" t="s">
         <v>63</v>
@@ -11530,8 +11530,8 @@
         <f t="shared" si="25"/>
         <v>j</v>
       </c>
-      <c r="J96">
-        <v>1</v>
+      <c r="J96" t="s">
+        <v>63</v>
       </c>
       <c r="K96" t="s">
         <v>63</v>
@@ -11639,8 +11639,8 @@
         <f t="shared" si="25"/>
         <v>f</v>
       </c>
-      <c r="J97">
-        <v>0</v>
+      <c r="J97" t="s">
+        <v>63</v>
       </c>
       <c r="K97" t="s">
         <v>63</v>
@@ -11748,8 +11748,8 @@
         <f t="shared" ref="I98:I109" si="36">IF(AND(Y98=1,O98=0),"f",IF(AND(Y98=1,O98=1),"j",IF(AND(Y98=0,O98=0),"j","f")))</f>
         <v>j</v>
       </c>
-      <c r="J98">
-        <v>1</v>
+      <c r="J98" t="s">
+        <v>63</v>
       </c>
       <c r="K98" t="s">
         <v>63</v>
@@ -11783,7 +11783,7 @@
         <v>14</v>
       </c>
       <c r="U98">
-        <f t="shared" ref="U98:U129" si="37">IF(O98=0,S98,T98)</f>
+        <f t="shared" ref="U98:U109" si="37">IF(O98=0,S98,T98)</f>
         <v>14</v>
       </c>
       <c r="V98">
@@ -11857,8 +11857,8 @@
         <f t="shared" si="36"/>
         <v>f</v>
       </c>
-      <c r="J99">
-        <v>0</v>
+      <c r="J99" t="s">
+        <v>63</v>
       </c>
       <c r="K99" t="s">
         <v>63</v>
@@ -11966,8 +11966,8 @@
         <f t="shared" si="36"/>
         <v>j</v>
       </c>
-      <c r="J100">
-        <v>0</v>
+      <c r="J100" t="s">
+        <v>63</v>
       </c>
       <c r="K100" t="s">
         <v>63</v>
@@ -11979,7 +11979,7 @@
         <v>1</v>
       </c>
       <c r="N100" t="str">
-        <f t="shared" ref="N100:N131" si="42">IF(AND(M100=1,M98=1),"REP2",IF(AND(M100=1,M97=1),"REP3","."))</f>
+        <f t="shared" ref="N100:N109" si="42">IF(AND(M100=1,M98=1),"REP2",IF(AND(M100=1,M97=1),"REP3","."))</f>
         <v>REP3</v>
       </c>
       <c r="O100">
@@ -12036,7 +12036,7 @@
         <v>49</v>
       </c>
       <c r="AE100" t="str">
-        <f t="shared" ref="AE100:AE131" si="43">IF(Q100=Q98,"REP2",IF(Q100=Q97,"REP3","."))</f>
+        <f t="shared" ref="AE100:AE109" si="43">IF(Q100=Q98,"REP2",IF(Q100=Q97,"REP3","."))</f>
         <v>.</v>
       </c>
       <c r="AF100">
@@ -12075,8 +12075,8 @@
         <f t="shared" si="36"/>
         <v>j</v>
       </c>
-      <c r="J101">
-        <v>0</v>
+      <c r="J101" t="s">
+        <v>63</v>
       </c>
       <c r="K101" t="s">
         <v>63</v>
@@ -12184,8 +12184,8 @@
         <f t="shared" si="36"/>
         <v>j</v>
       </c>
-      <c r="J102">
-        <v>0</v>
+      <c r="J102" t="s">
+        <v>63</v>
       </c>
       <c r="K102" t="s">
         <v>63</v>
@@ -12293,8 +12293,8 @@
         <f t="shared" si="36"/>
         <v>f</v>
       </c>
-      <c r="J103">
-        <v>0</v>
+      <c r="J103" t="s">
+        <v>63</v>
       </c>
       <c r="K103" t="s">
         <v>63</v>
@@ -12402,8 +12402,8 @@
         <f t="shared" si="36"/>
         <v>j</v>
       </c>
-      <c r="J104">
-        <v>0</v>
+      <c r="J104" t="s">
+        <v>63</v>
       </c>
       <c r="K104" t="s">
         <v>63</v>
@@ -12511,8 +12511,8 @@
         <f t="shared" si="36"/>
         <v>j</v>
       </c>
-      <c r="J105">
-        <v>0</v>
+      <c r="J105" t="s">
+        <v>63</v>
       </c>
       <c r="K105" t="s">
         <v>63</v>
@@ -12620,8 +12620,8 @@
         <f t="shared" si="36"/>
         <v>j</v>
       </c>
-      <c r="J106">
-        <v>0</v>
+      <c r="J106" t="s">
+        <v>63</v>
       </c>
       <c r="K106" t="s">
         <v>63</v>
@@ -12729,8 +12729,8 @@
         <f t="shared" si="36"/>
         <v>f</v>
       </c>
-      <c r="J107">
-        <v>0</v>
+      <c r="J107" t="s">
+        <v>63</v>
       </c>
       <c r="K107" t="s">
         <v>63</v>
@@ -12838,8 +12838,8 @@
         <f t="shared" si="36"/>
         <v>j</v>
       </c>
-      <c r="J108">
-        <v>1</v>
+      <c r="J108" t="s">
+        <v>63</v>
       </c>
       <c r="K108" t="s">
         <v>63</v>
@@ -12947,8 +12947,8 @@
         <f t="shared" si="36"/>
         <v>j</v>
       </c>
-      <c r="J109">
-        <v>0</v>
+      <c r="J109" t="s">
+        <v>63</v>
       </c>
       <c r="K109" t="s">
         <v>63</v>

</xml_diff>